<commit_message>
Battery PCB new gerber
</commit_message>
<xml_diff>
--- a/hardware/TIYCS_battery/TIYCS_battery-top-pos.xlsx
+++ b/hardware/TIYCS_battery/TIYCS_battery-top-pos.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="87">
   <si>
     <t>TIYCS_battery-top-pos</t>
   </si>
@@ -46,10 +46,10 @@
     <t>CP_Elec_10x10</t>
   </si>
   <si>
-    <t>15.000000</t>
-  </si>
-  <si>
-    <t>-89.330000</t>
+    <t>20.660000</t>
+  </si>
+  <si>
+    <t>-89.190000</t>
   </si>
   <si>
     <t>0.000000</t>
@@ -100,7 +100,25 @@
     <t>C_Elec_10x10.2</t>
   </si>
   <si>
-    <t>85.000000</t>
+    <t>69.610000</t>
+  </si>
+  <si>
+    <t>-84.950000</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C_Polarized</t>
+  </si>
+  <si>
+    <t>CP_Radial_D12.5mm_P5.00mm</t>
+  </si>
+  <si>
+    <t>6.960000</t>
+  </si>
+  <si>
+    <t>-36.806041</t>
   </si>
   <si>
     <t>D1</t>
@@ -118,6 +136,9 @@
     <t>-73.570000</t>
   </si>
   <si>
+    <t>90.000000</t>
+  </si>
+  <si>
     <t>D2</t>
   </si>
   <si>
@@ -136,24 +157,6 @@
     <t>180.000000</t>
   </si>
   <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>1N4148</t>
-  </si>
-  <si>
-    <t>D_SOD-323F</t>
-  </si>
-  <si>
-    <t>29.810000</t>
-  </si>
-  <si>
-    <t>-94.920000</t>
-  </si>
-  <si>
-    <t>90.000000</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
@@ -163,10 +166,10 @@
     <t>BarrelJack_CLIFF_FC681465S_SMT_Horizontal</t>
   </si>
   <si>
-    <t>6.400000</t>
-  </si>
-  <si>
-    <t>-50.000000</t>
+    <t>84.810000</t>
+  </si>
+  <si>
+    <t>-91.510000</t>
   </si>
   <si>
     <t>J2</t>
@@ -178,10 +181,25 @@
     <t>TerminalBlock_Altech_AK300-2_P5.00mm</t>
   </si>
   <si>
-    <t>6.300000</t>
-  </si>
-  <si>
-    <t>-77.580000</t>
+    <t>6.560000</t>
+  </si>
+  <si>
+    <t>-87.220000</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>XT60PW-M</t>
+  </si>
+  <si>
+    <t>AMASS_XT60PW-M</t>
+  </si>
+  <si>
+    <t>5.530000</t>
+  </si>
+  <si>
+    <t>-66.870000</t>
   </si>
   <si>
     <t>L1</t>
@@ -199,21 +217,12 @@
     <t>-79.177500</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>10K</t>
-  </si>
-  <si>
-    <t>69.890000</t>
-  </si>
-  <si>
-    <t>-98.250000</t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
+    <t>13K</t>
+  </si>
+  <si>
     <t>69.970000</t>
   </si>
   <si>
@@ -223,7 +232,10 @@
     <t>R3</t>
   </si>
   <si>
-    <t>3.3K</t>
+    <t>1.5K</t>
+  </si>
+  <si>
+    <t>R_0805_2012Metric</t>
   </si>
   <si>
     <t>74.030000</t>
@@ -241,10 +253,10 @@
     <t>MR1-110-C5N-BB</t>
   </si>
   <si>
-    <t>6.830000</t>
-  </si>
-  <si>
-    <t>-32.610000</t>
+    <t>6.690000</t>
+  </si>
+  <si>
+    <t>-25.380000</t>
   </si>
   <si>
     <t>U3</t>
@@ -287,7 +299,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -306,14 +318,8 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="15"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -333,36 +339,6 @@
       </top>
       <bottom style="thin">
         <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="14"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="14"/>
       </bottom>
       <diagonal/>
     </border>
@@ -389,7 +365,7 @@
         <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
         <color indexed="13"/>
@@ -404,7 +380,7 @@
         <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
         <color indexed="13"/>
@@ -462,7 +438,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -478,28 +454,22 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -522,10 +492,9 @@
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1614,394 +1583,394 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" ht="20.7" customHeight="1">
+    <row r="2" ht="14.7" customHeight="1">
       <c r="A2" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" t="s" s="3">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="5">
+      <c r="C2" t="s" s="3">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="5">
+      <c r="D2" t="s" s="3">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="5">
+      <c r="E2" t="s" s="3">
         <v>5</v>
       </c>
-      <c r="F2" t="s" s="5">
+      <c r="F2" t="s" s="3">
         <v>6</v>
       </c>
-      <c r="G2" t="s" s="5">
+      <c r="G2" t="s" s="3">
         <v>7</v>
       </c>
     </row>
     <row r="3" ht="20.35" customHeight="1">
-      <c r="A3" t="s" s="6">
+      <c r="A3" t="s" s="4">
         <v>8</v>
       </c>
-      <c r="B3" t="s" s="7">
+      <c r="B3" t="s" s="5">
         <v>9</v>
       </c>
-      <c r="C3" t="s" s="8">
+      <c r="C3" t="s" s="6">
         <v>10</v>
       </c>
-      <c r="D3" t="s" s="8">
+      <c r="D3" t="s" s="6">
         <v>11</v>
       </c>
-      <c r="E3" t="s" s="8">
+      <c r="E3" t="s" s="6">
         <v>12</v>
       </c>
-      <c r="F3" t="s" s="8">
+      <c r="F3" t="s" s="6">
         <v>13</v>
       </c>
-      <c r="G3" t="s" s="8">
+      <c r="G3" t="s" s="6">
         <v>14</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="9">
+      <c r="A4" t="s" s="7">
         <v>15</v>
       </c>
-      <c r="B4" t="s" s="10">
+      <c r="B4" t="s" s="8">
         <v>16</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="9">
         <v>805</v>
       </c>
-      <c r="D4" t="s" s="12">
+      <c r="D4" t="s" s="10">
         <v>17</v>
       </c>
-      <c r="E4" t="s" s="12">
+      <c r="E4" t="s" s="10">
         <v>18</v>
       </c>
-      <c r="F4" t="s" s="12">
+      <c r="F4" t="s" s="10">
         <v>13</v>
       </c>
-      <c r="G4" t="s" s="12">
+      <c r="G4" t="s" s="10">
         <v>14</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="9">
+      <c r="A5" t="s" s="7">
         <v>19</v>
       </c>
-      <c r="B5" t="s" s="10">
+      <c r="B5" t="s" s="8">
         <v>16</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="9">
         <v>805</v>
       </c>
-      <c r="D5" t="s" s="12">
+      <c r="D5" t="s" s="10">
         <v>20</v>
       </c>
-      <c r="E5" t="s" s="12">
+      <c r="E5" t="s" s="10">
         <v>21</v>
       </c>
-      <c r="F5" t="s" s="12">
+      <c r="F5" t="s" s="10">
         <v>22</v>
       </c>
-      <c r="G5" t="s" s="12">
+      <c r="G5" t="s" s="10">
         <v>14</v>
       </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="9">
+      <c r="A6" t="s" s="7">
         <v>23</v>
       </c>
-      <c r="B6" t="s" s="10">
+      <c r="B6" t="s" s="8">
         <v>16</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="9">
         <v>805</v>
       </c>
-      <c r="D6" t="s" s="12">
+      <c r="D6" t="s" s="10">
         <v>24</v>
       </c>
-      <c r="E6" t="s" s="12">
+      <c r="E6" t="s" s="10">
         <v>25</v>
       </c>
-      <c r="F6" t="s" s="12">
+      <c r="F6" t="s" s="10">
         <v>22</v>
       </c>
-      <c r="G6" t="s" s="12">
+      <c r="G6" t="s" s="10">
         <v>14</v>
       </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="9">
+      <c r="A7" t="s" s="7">
         <v>26</v>
       </c>
-      <c r="B7" t="s" s="10">
+      <c r="B7" t="s" s="8">
         <v>27</v>
       </c>
-      <c r="C7" t="s" s="12">
+      <c r="C7" t="s" s="10">
         <v>28</v>
       </c>
-      <c r="D7" t="s" s="12">
+      <c r="D7" t="s" s="10">
         <v>29</v>
       </c>
-      <c r="E7" t="s" s="12">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s" s="12">
+      <c r="E7" t="s" s="10">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s" s="10">
         <v>13</v>
       </c>
-      <c r="G7" t="s" s="12">
+      <c r="G7" t="s" s="10">
         <v>14</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="9">
-        <v>30</v>
-      </c>
-      <c r="B8" t="s" s="10">
+      <c r="A8" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="C8" t="s" s="12">
+      <c r="B8" t="s" s="8">
         <v>32</v>
       </c>
-      <c r="D8" t="s" s="12">
+      <c r="C8" t="s" s="10">
         <v>33</v>
       </c>
-      <c r="E8" t="s" s="12">
+      <c r="D8" t="s" s="10">
         <v>34</v>
       </c>
-      <c r="F8" t="s" s="12">
+      <c r="E8" t="s" s="10">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s" s="10">
         <v>22</v>
       </c>
-      <c r="G8" t="s" s="12">
+      <c r="G8" t="s" s="10">
         <v>14</v>
       </c>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="9">
-        <v>35</v>
-      </c>
-      <c r="B9" t="s" s="10">
+      <c r="A9" t="s" s="7">
         <v>36</v>
       </c>
-      <c r="C9" t="s" s="12">
+      <c r="B9" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="D9" t="s" s="12">
+      <c r="C9" t="s" s="10">
         <v>38</v>
       </c>
-      <c r="E9" t="s" s="12">
+      <c r="D9" t="s" s="10">
         <v>39</v>
       </c>
-      <c r="F9" t="s" s="12">
+      <c r="E9" t="s" s="10">
         <v>40</v>
       </c>
-      <c r="G9" t="s" s="12">
+      <c r="F9" t="s" s="10">
+        <v>41</v>
+      </c>
+      <c r="G9" t="s" s="10">
         <v>14</v>
       </c>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="9">
-        <v>41</v>
-      </c>
-      <c r="B10" t="s" s="10">
+      <c r="A10" t="s" s="7">
         <v>42</v>
       </c>
-      <c r="C10" t="s" s="12">
+      <c r="B10" t="s" s="8">
         <v>43</v>
       </c>
-      <c r="D10" t="s" s="12">
+      <c r="C10" t="s" s="10">
         <v>44</v>
       </c>
-      <c r="E10" t="s" s="12">
+      <c r="D10" t="s" s="10">
         <v>45</v>
       </c>
-      <c r="F10" t="s" s="12">
+      <c r="E10" t="s" s="10">
         <v>46</v>
       </c>
-      <c r="G10" t="s" s="12">
+      <c r="F10" t="s" s="10">
+        <v>47</v>
+      </c>
+      <c r="G10" t="s" s="10">
         <v>14</v>
       </c>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" t="s" s="9">
-        <v>47</v>
-      </c>
-      <c r="B11" t="s" s="10">
+      <c r="A11" t="s" s="7">
         <v>48</v>
       </c>
-      <c r="C11" t="s" s="12">
+      <c r="B11" t="s" s="8">
         <v>49</v>
       </c>
-      <c r="D11" t="s" s="12">
+      <c r="C11" t="s" s="10">
         <v>50</v>
       </c>
-      <c r="E11" t="s" s="12">
+      <c r="D11" t="s" s="10">
         <v>51</v>
       </c>
-      <c r="F11" t="s" s="12">
-        <v>13</v>
-      </c>
-      <c r="G11" t="s" s="12">
+      <c r="E11" t="s" s="10">
+        <v>52</v>
+      </c>
+      <c r="F11" t="s" s="10">
+        <v>41</v>
+      </c>
+      <c r="G11" t="s" s="10">
         <v>14</v>
       </c>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="9">
-        <v>52</v>
-      </c>
-      <c r="B12" t="s" s="10">
+      <c r="A12" t="s" s="7">
         <v>53</v>
       </c>
-      <c r="C12" t="s" s="12">
+      <c r="B12" t="s" s="8">
         <v>54</v>
       </c>
-      <c r="D12" t="s" s="12">
+      <c r="C12" t="s" s="10">
         <v>55</v>
       </c>
-      <c r="E12" t="s" s="12">
+      <c r="D12" t="s" s="10">
         <v>56</v>
       </c>
-      <c r="F12" t="s" s="12">
-        <v>46</v>
-      </c>
-      <c r="G12" t="s" s="12">
+      <c r="E12" t="s" s="10">
+        <v>57</v>
+      </c>
+      <c r="F12" t="s" s="10">
+        <v>41</v>
+      </c>
+      <c r="G12" t="s" s="10">
         <v>14</v>
       </c>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" t="s" s="9">
-        <v>57</v>
-      </c>
-      <c r="B13" t="s" s="10">
+      <c r="A13" t="s" s="7">
         <v>58</v>
       </c>
-      <c r="C13" t="s" s="12">
+      <c r="B13" t="s" s="8">
         <v>59</v>
       </c>
-      <c r="D13" t="s" s="12">
+      <c r="C13" t="s" s="10">
         <v>60</v>
       </c>
-      <c r="E13" t="s" s="12">
+      <c r="D13" t="s" s="10">
         <v>61</v>
       </c>
-      <c r="F13" t="s" s="12">
-        <v>13</v>
-      </c>
-      <c r="G13" t="s" s="12">
+      <c r="E13" t="s" s="10">
+        <v>62</v>
+      </c>
+      <c r="F13" t="s" s="10">
+        <v>41</v>
+      </c>
+      <c r="G13" t="s" s="10">
         <v>14</v>
       </c>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" t="s" s="9">
-        <v>62</v>
-      </c>
-      <c r="B14" t="s" s="10">
+      <c r="A14" t="s" s="7">
         <v>63</v>
       </c>
-      <c r="C14" s="11">
-        <v>805</v>
-      </c>
-      <c r="D14" t="s" s="12">
+      <c r="B14" t="s" s="8">
         <v>64</v>
       </c>
-      <c r="E14" t="s" s="12">
+      <c r="C14" t="s" s="10">
         <v>65</v>
       </c>
-      <c r="F14" t="s" s="12">
+      <c r="D14" t="s" s="10">
+        <v>66</v>
+      </c>
+      <c r="E14" t="s" s="10">
+        <v>67</v>
+      </c>
+      <c r="F14" t="s" s="10">
         <v>13</v>
       </c>
-      <c r="G14" t="s" s="12">
+      <c r="G14" t="s" s="10">
         <v>14</v>
       </c>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" t="s" s="9">
-        <v>66</v>
-      </c>
-      <c r="B15" t="s" s="10">
-        <v>63</v>
-      </c>
-      <c r="C15" s="11">
+      <c r="A15" t="s" s="7">
+        <v>68</v>
+      </c>
+      <c r="B15" t="s" s="8">
+        <v>69</v>
+      </c>
+      <c r="C15" s="9">
         <v>805</v>
       </c>
-      <c r="D15" t="s" s="12">
-        <v>67</v>
-      </c>
-      <c r="E15" t="s" s="12">
-        <v>68</v>
-      </c>
-      <c r="F15" t="s" s="12">
+      <c r="D15" t="s" s="10">
+        <v>70</v>
+      </c>
+      <c r="E15" t="s" s="10">
+        <v>71</v>
+      </c>
+      <c r="F15" t="s" s="10">
         <v>13</v>
       </c>
-      <c r="G15" t="s" s="12">
+      <c r="G15" t="s" s="10">
         <v>14</v>
       </c>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" t="s" s="9">
-        <v>69</v>
-      </c>
-      <c r="B16" t="s" s="10">
-        <v>70</v>
-      </c>
-      <c r="C16" s="11">
-        <v>805</v>
-      </c>
-      <c r="D16" t="s" s="12">
-        <v>71</v>
-      </c>
-      <c r="E16" t="s" s="12">
+      <c r="A16" t="s" s="7">
         <v>72</v>
       </c>
-      <c r="F16" t="s" s="12">
+      <c r="B16" t="s" s="8">
+        <v>73</v>
+      </c>
+      <c r="C16" t="s" s="10">
+        <v>74</v>
+      </c>
+      <c r="D16" t="s" s="10">
+        <v>75</v>
+      </c>
+      <c r="E16" t="s" s="10">
+        <v>76</v>
+      </c>
+      <c r="F16" t="s" s="10">
         <v>13</v>
       </c>
-      <c r="G16" t="s" s="12">
+      <c r="G16" t="s" s="10">
         <v>14</v>
       </c>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" t="s" s="9">
-        <v>73</v>
-      </c>
-      <c r="B17" t="s" s="10">
-        <v>74</v>
-      </c>
-      <c r="C17" t="s" s="12">
-        <v>75</v>
-      </c>
-      <c r="D17" t="s" s="12">
-        <v>76</v>
-      </c>
-      <c r="E17" t="s" s="12">
+      <c r="A17" t="s" s="7">
         <v>77</v>
       </c>
-      <c r="F17" t="s" s="12">
-        <v>46</v>
-      </c>
-      <c r="G17" t="s" s="12">
+      <c r="B17" t="s" s="8">
+        <v>78</v>
+      </c>
+      <c r="C17" t="s" s="10">
+        <v>79</v>
+      </c>
+      <c r="D17" t="s" s="10">
+        <v>80</v>
+      </c>
+      <c r="E17" t="s" s="10">
+        <v>81</v>
+      </c>
+      <c r="F17" t="s" s="10">
+        <v>41</v>
+      </c>
+      <c r="G17" t="s" s="10">
         <v>14</v>
       </c>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" t="s" s="9">
-        <v>78</v>
-      </c>
-      <c r="B18" t="s" s="10">
-        <v>79</v>
-      </c>
-      <c r="C18" t="s" s="12">
-        <v>80</v>
-      </c>
-      <c r="D18" t="s" s="12">
-        <v>81</v>
-      </c>
-      <c r="E18" t="s" s="12">
+      <c r="A18" t="s" s="7">
         <v>82</v>
       </c>
-      <c r="F18" t="s" s="12">
-        <v>46</v>
-      </c>
-      <c r="G18" t="s" s="12">
+      <c r="B18" t="s" s="8">
+        <v>83</v>
+      </c>
+      <c r="C18" t="s" s="10">
+        <v>84</v>
+      </c>
+      <c r="D18" t="s" s="10">
+        <v>85</v>
+      </c>
+      <c r="E18" t="s" s="10">
+        <v>86</v>
+      </c>
+      <c r="F18" t="s" s="10">
+        <v>41</v>
+      </c>
+      <c r="G18" t="s" s="10">
         <v>14</v>
       </c>
     </row>

</xml_diff>